<commit_message>
save date range imput
</commit_message>
<xml_diff>
--- a/sales.xlsx
+++ b/sales.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:S1006"/>
+  <dimension ref="B2:S1007"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -70637,74 +70637,146 @@
       </c>
     </row>
     <row r="1006">
-      <c r="B1006" t="inlineStr">
+      <c r="B1006" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C1006" t="inlineStr">
+      <c r="C1006" s="0" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D1006" t="inlineStr">
+      <c r="D1006" s="0" t="inlineStr">
         <is>
           <t>Berlin</t>
         </is>
       </c>
-      <c r="E1006" t="inlineStr">
+      <c r="E1006" s="0" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
-      <c r="F1006" t="inlineStr">
+      <c r="F1006" s="0" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="G1006" t="inlineStr">
+      <c r="G1006" s="0" t="inlineStr">
         <is>
           <t>Health and beauty</t>
         </is>
       </c>
-      <c r="H1006" t="n">
+      <c r="H1006" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="I1006" t="n">
+      <c r="I1006" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="J1006" t="n">
+      <c r="J1006" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="K1006" t="n">
+      <c r="K1006" s="0" t="n">
         <v>231</v>
       </c>
       <c r="L1006" s="14" t="n">
         <v>45798</v>
       </c>
-      <c r="M1006" t="inlineStr">
+      <c r="M1006" s="0" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>
       </c>
-      <c r="N1006" t="inlineStr">
+      <c r="N1006" s="0" t="inlineStr">
         <is>
           <t>Ewallet</t>
         </is>
       </c>
-      <c r="O1006" t="n">
+      <c r="O1006" s="0" t="n">
         <v>220</v>
       </c>
-      <c r="P1006" t="n">
+      <c r="P1006" s="0" t="n">
         <v>4.7619</v>
       </c>
-      <c r="Q1006" t="n">
+      <c r="Q1006" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="R1006" t="n">
+      <c r="R1006" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="S1006" t="n">
+      <c r="S1006" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>1111-11-111</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D1007" t="inlineStr">
+        <is>
+          <t>Berlin</t>
+        </is>
+      </c>
+      <c r="E1007" t="inlineStr">
+        <is>
+          <t>Member</t>
+        </is>
+      </c>
+      <c r="F1007" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="G1007" t="inlineStr">
+        <is>
+          <t>Health and beauty</t>
+        </is>
+      </c>
+      <c r="H1007" t="n">
+        <v>33</v>
+      </c>
+      <c r="I1007" t="n">
+        <v>5</v>
+      </c>
+      <c r="J1007" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="K1007" t="n">
+        <v>173.25</v>
+      </c>
+      <c r="L1007" s="14" t="n">
+        <v>45801</v>
+      </c>
+      <c r="M1007" t="inlineStr">
+        <is>
+          <t>15:03:00</t>
+        </is>
+      </c>
+      <c r="N1007" t="inlineStr">
+        <is>
+          <t>Ewallet</t>
+        </is>
+      </c>
+      <c r="O1007" t="n">
+        <v>165</v>
+      </c>
+      <c r="P1007" t="n">
+        <v>4.7619</v>
+      </c>
+      <c r="Q1007" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="R1007" t="n">
+        <v>10</v>
+      </c>
+      <c r="S1007" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>